<commit_message>
Apparently LED on PC13 is interfering, changed pinout
</commit_message>
<xml_diff>
--- a/doc/Pinout.xlsx
+++ b/doc/Pinout.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\stm32f103-midi\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D21B86-7664-4901-8C53-2AE739780218}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E641E9-AD76-4432-834B-FE747D16513A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="855" windowWidth="19440" windowHeight="15600" xr2:uid="{F16473F9-5855-4B57-A77B-826CCC8D5F08}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>G</t>
   </si>
@@ -39,62 +39,65 @@
     <t>3.3V</t>
   </si>
   <si>
-    <t>R</t>
+    <t>B12</t>
   </si>
   <si>
-    <t>B11</t>
+    <t>B13</t>
   </si>
   <si>
-    <t>B10</t>
+    <t>B14</t>
   </si>
   <si>
-    <t>B1</t>
+    <t>B15</t>
   </si>
   <si>
-    <t>B0</t>
+    <t>A8</t>
   </si>
   <si>
-    <t>A7</t>
+    <t>A9</t>
   </si>
   <si>
-    <t>A6</t>
+    <t>A10</t>
   </si>
   <si>
-    <t>A5</t>
+    <t>A11</t>
   </si>
   <si>
-    <t>A4</t>
+    <t>A12</t>
   </si>
   <si>
-    <t>A3</t>
+    <t>A15</t>
   </si>
   <si>
-    <t>A2</t>
+    <t>B3</t>
   </si>
   <si>
-    <t>A1</t>
+    <t>B4</t>
   </si>
   <si>
-    <t>A0</t>
+    <t>B5</t>
   </si>
   <si>
-    <t>C15</t>
+    <t>B6</t>
   </si>
   <si>
-    <t>C14</t>
+    <t>B7</t>
   </si>
   <si>
-    <t>C13</t>
+    <t>B8</t>
   </si>
   <si>
-    <t>VB</t>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>5V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +120,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -132,7 +141,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -155,11 +164,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -177,6 +195,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -200,13 +225,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>230606</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>105276</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>240631</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>25066</xdr:rowOff>
@@ -245,13 +270,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>225592</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>100263</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>230606</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>10027</xdr:rowOff>
@@ -290,13 +315,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>225591</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>230605</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>5014</xdr:rowOff>
@@ -335,13 +360,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>220579</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>110289</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>225593</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>20053</xdr:rowOff>
@@ -380,16 +405,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>210553</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>210554</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>145381</xdr:colOff>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>149679</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>5013</xdr:rowOff>
+      <xdr:rowOff>4536</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -404,8 +429,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="4035592" y="2476500"/>
-          <a:ext cx="2737184" cy="5013"/>
+          <a:off x="3553375" y="2476501"/>
+          <a:ext cx="3898804" cy="4535"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -430,16 +455,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>150395</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>181429</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>283351</xdr:colOff>
+      <xdr:rowOff>4536</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>149679</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>2614</xdr:rowOff>
+      <xdr:rowOff>4537</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -454,8 +479,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="2922671" y="1714500"/>
-          <a:ext cx="2489141" cy="2614"/>
+          <a:off x="3524250" y="1719036"/>
+          <a:ext cx="3356429" cy="1"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -480,16 +505,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>145382</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47627</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>242968</xdr:colOff>
+      <xdr:rowOff>4536</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>145145</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>2336</xdr:rowOff>
+      <xdr:rowOff>5821</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -500,12 +525,14 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="138" idx="1"/>
+        </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="2631908" y="2095500"/>
-          <a:ext cx="2739521" cy="2336"/>
+        <a:xfrm flipH="1">
+          <a:off x="3390448" y="2100036"/>
+          <a:ext cx="3771447" cy="1285"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -530,13 +557,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>125329</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>122374</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>5957</xdr:rowOff>
@@ -580,13 +607,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>215565</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>115303</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>222782</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>66147</xdr:rowOff>
@@ -627,13 +654,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>390526</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
@@ -698,13 +725,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>400051</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
@@ -769,16 +796,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>145382</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>172358</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>230605</xdr:colOff>
+      <xdr:colOff>149679</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>5013</xdr:rowOff>
+      <xdr:rowOff>4536</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -792,9 +819,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="2346158" y="2857500"/>
-          <a:ext cx="3494171" cy="5013"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3515179" y="2857500"/>
+          <a:ext cx="4222750" cy="4536"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -819,13 +846,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>52917</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>52918</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>395818</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>119592</xdr:rowOff>
@@ -890,13 +917,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>57151</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>400052</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>114299</xdr:rowOff>
@@ -961,13 +988,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>46038</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>50272</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>388939</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>116946</xdr:rowOff>
@@ -1032,13 +1059,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>47626</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>78317</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>390527</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>144991</xdr:rowOff>
@@ -1103,13 +1130,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>57151</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>78317</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>400052</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>144991</xdr:rowOff>
@@ -1174,13 +1201,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>52918</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>74085</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>395819</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>140759</xdr:rowOff>
@@ -1245,13 +1272,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>57152</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>68792</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>400053</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>135466</xdr:rowOff>
@@ -1316,13 +1343,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>46039</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>71439</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>388940</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>138113</xdr:rowOff>
@@ -1387,13 +1414,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>47627</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>67734</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>390528</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>134408</xdr:rowOff>
@@ -1458,13 +1485,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>57152</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>67734</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>400053</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>134408</xdr:rowOff>
@@ -1529,13 +1556,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>52919</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>63502</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>395820</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>130176</xdr:rowOff>
@@ -1600,13 +1627,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>57153</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>58209</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>400054</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>124883</xdr:rowOff>
@@ -1671,13 +1698,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>46040</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>60856</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>388941</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>127530</xdr:rowOff>
@@ -1742,13 +1769,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>42335</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>62442</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>385236</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>129116</xdr:rowOff>
@@ -1813,13 +1840,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>51860</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>62442</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>394761</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>129116</xdr:rowOff>
@@ -1884,13 +1911,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>47627</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>58210</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>390528</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>124884</xdr:rowOff>
@@ -1955,13 +1982,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>51861</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>52917</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>394762</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>119591</xdr:rowOff>
@@ -2026,13 +2053,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>40748</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>55564</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>383649</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>122238</xdr:rowOff>
@@ -2097,13 +2124,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>52918</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>73025</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>395819</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>139699</xdr:rowOff>
@@ -2168,13 +2195,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>62443</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>73025</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>405344</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>139699</xdr:rowOff>
@@ -2239,13 +2266,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>58210</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>68793</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>401111</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>135467</xdr:rowOff>
@@ -2310,13 +2337,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>62444</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>405345</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>130174</xdr:rowOff>
@@ -2381,13 +2408,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>51331</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>66147</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>394232</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>132821</xdr:rowOff>
@@ -2452,13 +2479,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>125330</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>105275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>130343</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
@@ -2497,16 +2524,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>145382</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>140368</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>115302</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>145384</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>145143</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>9071</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2521,8 +2548,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2917658" y="686802"/>
-          <a:ext cx="2" cy="1027697"/>
+          <a:off x="6871368" y="686802"/>
+          <a:ext cx="4775" cy="1036769"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2542,16 +2569,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>145381</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>136071</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>120316</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>155410</xdr:colOff>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>140849</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>185487</xdr:rowOff>
+      <xdr:rowOff>190022</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2565,9 +2592,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="2631907" y="691816"/>
-          <a:ext cx="10029" cy="1398671"/>
+        <a:xfrm>
+          <a:off x="7152821" y="680357"/>
+          <a:ext cx="4778" cy="1414665"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2587,16 +2614,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>140369</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>144905</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>110290</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>150400</xdr:colOff>
+      <xdr:rowOff>99786</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>145143</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>185487</xdr:rowOff>
+      <xdr:rowOff>190023</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2611,8 +2638,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="2341145" y="681790"/>
-          <a:ext cx="10031" cy="2170697"/>
+          <a:off x="7733155" y="671286"/>
+          <a:ext cx="238" cy="2185737"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2632,16 +2659,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>140374</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>136071</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>145381</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>10026</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>186919</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2656,8 +2683,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6767769" y="666750"/>
-          <a:ext cx="5007" cy="1819776"/>
+          <a:off x="7438571" y="680357"/>
+          <a:ext cx="9310" cy="1792562"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2677,16 +2704,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>150395</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>185486</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>240632</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>62944</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>149680</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>6098</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2697,12 +2724,14 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="76" idx="1"/>
+        </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="2065421" y="3233486"/>
-          <a:ext cx="3784935" cy="5014"/>
+          <a:off x="3405765" y="3238500"/>
+          <a:ext cx="4617915" cy="6098"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2727,13 +2756,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>62944</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>68011</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>405845</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>134685</xdr:rowOff>
@@ -2798,13 +2827,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>72469</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>68011</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>415370</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>134685</xdr:rowOff>
@@ -2869,13 +2898,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>68236</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>63779</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>411137</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>130453</xdr:rowOff>
@@ -2940,13 +2969,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>72470</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>58486</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>415371</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>125160</xdr:rowOff>
@@ -3011,13 +3040,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>61357</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>61133</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>404258</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>127807</xdr:rowOff>
@@ -3082,14 +3111,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>140374</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>149918</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>105276</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>145382</xdr:colOff>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -3105,9 +3134,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2055400" y="676776"/>
-          <a:ext cx="5008" cy="2561724"/>
+        <a:xfrm flipH="1">
+          <a:off x="8023918" y="680357"/>
+          <a:ext cx="8832" cy="2558143"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3127,16 +3156,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>140369</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>185486</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>240627</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>62938</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>5013</xdr:rowOff>
+      <xdr:rowOff>4536</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>140607</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>6098</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3147,12 +3176,14 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="91" idx="1"/>
+        </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="1769645" y="3614486"/>
-          <a:ext cx="4080706" cy="10027"/>
+          <a:off x="3405759" y="3624036"/>
+          <a:ext cx="4894598" cy="1562"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3177,13 +3208,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>62938</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>68011</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>405839</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>134685</xdr:rowOff>
@@ -3248,13 +3279,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>72463</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>68011</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>415364</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>134685</xdr:rowOff>
@@ -3319,13 +3350,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>68230</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>63779</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>411131</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>130453</xdr:rowOff>
@@ -3390,13 +3421,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>72464</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>58486</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>415365</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>125160</xdr:rowOff>
@@ -3461,16 +3492,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>140369</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>140368</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>105276</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>145382</xdr:colOff>
+      <xdr:rowOff>109811</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>145381</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>4535</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3485,7 +3516,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="1769645" y="676776"/>
+          <a:off x="8300118" y="681311"/>
           <a:ext cx="5013" cy="2942724"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3506,13 +3537,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>70184</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>55145</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>413085</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>121819</xdr:rowOff>
@@ -3577,16 +3608,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>145382</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>185486</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>245640</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>67951</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>4536</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>145144</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>6098</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3597,12 +3628,14 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="100" idx="1"/>
+        </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="1488908" y="3995486"/>
-          <a:ext cx="4366456" cy="5014"/>
+          <a:off x="3410772" y="4005036"/>
+          <a:ext cx="5179872" cy="1562"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3627,13 +3660,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>67951</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>68011</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>410852</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>134685</xdr:rowOff>
@@ -3695,13 +3728,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>77476</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>68011</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>420377</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>134685</xdr:rowOff>
@@ -3763,13 +3796,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>73243</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>63779</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>416144</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>130453</xdr:rowOff>
@@ -3831,13 +3864,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>77477</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>58486</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>420378</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>125160</xdr:rowOff>
@@ -3902,13 +3935,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>75197</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>55145</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>418098</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>121819</xdr:rowOff>
@@ -3973,16 +4006,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>140369</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>140368</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>100264</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>155409</xdr:colOff>
+      <xdr:rowOff>95728</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>155408</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>5013</xdr:rowOff>
+      <xdr:rowOff>477</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3997,7 +4030,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="1483895" y="671764"/>
+          <a:off x="8585868" y="667228"/>
           <a:ext cx="15040" cy="3333749"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -4316,188 +4349,192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E534349B-027D-42B1-847A-CDE6C82C41D9}">
-  <dimension ref="B1:U4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="12" width="4.28515625" customWidth="1"/>
-    <col min="13" max="17" width="6.7109375" customWidth="1"/>
-    <col min="18" max="21" width="4.28515625" customWidth="1"/>
+    <col min="1" max="4" width="4.28515625" customWidth="1"/>
+    <col min="5" max="9" width="6.7109375" customWidth="1"/>
+    <col min="10" max="21" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="6">
+        <v>1</v>
+      </c>
       <c r="B1" s="6">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6">
+        <v>3</v>
+      </c>
+      <c r="D1" s="6">
+        <v>4</v>
+      </c>
+      <c r="E1" s="6">
+        <v>5</v>
+      </c>
+      <c r="F1" s="6">
+        <v>6</v>
+      </c>
+      <c r="G1" s="6">
+        <v>7</v>
+      </c>
+      <c r="H1" s="6">
+        <v>8</v>
+      </c>
+      <c r="I1" s="6">
+        <v>9</v>
+      </c>
+      <c r="J1" s="6">
+        <v>10</v>
+      </c>
+      <c r="K1" s="6">
+        <v>11</v>
+      </c>
+      <c r="L1" s="6">
+        <v>12</v>
+      </c>
+      <c r="M1" s="6">
+        <v>13</v>
+      </c>
+      <c r="N1" s="6">
+        <v>14</v>
+      </c>
+      <c r="O1" s="6">
+        <v>15</v>
+      </c>
+      <c r="P1" s="6">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="6">
+        <v>17</v>
+      </c>
+      <c r="R1" s="6">
+        <v>18</v>
+      </c>
+      <c r="S1" s="6">
+        <v>19</v>
+      </c>
+      <c r="T1" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5">
+        <v>5</v>
+      </c>
+      <c r="F2" s="5">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5">
+        <v>3</v>
+      </c>
+      <c r="H2" s="5">
+        <v>2</v>
+      </c>
+      <c r="I2" s="5">
         <v>1</v>
       </c>
-      <c r="C1" s="6">
-        <v>2</v>
-      </c>
-      <c r="D1" s="6">
-        <v>3</v>
-      </c>
-      <c r="E1" s="6">
-        <v>4</v>
-      </c>
-      <c r="F1" s="6">
-        <v>5</v>
-      </c>
-      <c r="G1" s="6">
-        <v>6</v>
-      </c>
-      <c r="H1" s="6">
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="9"/>
+      <c r="N2" s="5">
         <v>7</v>
       </c>
-      <c r="I1" s="6">
+      <c r="O2" s="5">
         <v>8</v>
       </c>
-      <c r="J1" s="6">
+      <c r="P2" s="5">
         <v>9</v>
       </c>
-      <c r="K1" s="6">
+      <c r="Q2" s="5">
         <v>10</v>
       </c>
-      <c r="L1" s="6">
+      <c r="R2" s="5">
         <v>11</v>
       </c>
-      <c r="M1" s="6">
+      <c r="S2" s="5">
         <v>12</v>
       </c>
-      <c r="N1" s="6">
+      <c r="T2" s="5">
         <v>13</v>
       </c>
-      <c r="O1" s="6">
-        <v>14</v>
-      </c>
-      <c r="P1" s="6">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="6">
-        <v>16</v>
-      </c>
-      <c r="R1" s="6">
-        <v>17</v>
-      </c>
-      <c r="S1" s="6">
-        <v>18</v>
-      </c>
-      <c r="T1" s="6">
-        <v>19</v>
-      </c>
-      <c r="U1" s="6">
-        <v>20</v>
-      </c>
     </row>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="F2" s="5">
-        <v>13</v>
-      </c>
-      <c r="G2" s="5">
-        <v>12</v>
-      </c>
-      <c r="H2" s="5">
-        <v>11</v>
-      </c>
-      <c r="I2" s="5">
-        <v>10</v>
-      </c>
-      <c r="J2" s="5">
-        <v>8</v>
-      </c>
-      <c r="K2" s="5">
-        <v>7</v>
-      </c>
-      <c r="L2" s="5">
-        <v>6</v>
-      </c>
-      <c r="M2" s="5">
-        <v>5</v>
-      </c>
-      <c r="N2" s="5">
-        <v>4</v>
-      </c>
-      <c r="O2" s="5">
-        <v>3</v>
-      </c>
-      <c r="P2" s="5">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="5">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="T3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -4517,7 +4554,6 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>